<commit_message>
Sharpe ratio calculated and reported in the notebooks
</commit_message>
<xml_diff>
--- a/Excel filies/evaluations.xlsx
+++ b/Excel filies/evaluations.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mac/PycharmProjects/algo_trading_system/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mac/PycharmProjects/algo_trading_system/Excel filies/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA3ABAFB-209C-AD4B-B8C8-BAA05ECDAC68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94889D54-185C-4A46-BB59-F8D3A02411C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="18840" xr2:uid="{0E26818A-CB76-4D45-87E0-C35511F6C792}"/>
   </bookViews>
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="34">
   <si>
     <t>State representation</t>
   </si>
@@ -168,6 +168,9 @@
   </si>
   <si>
     <t>[Low, High, Close, Sentiment, 8 Technical indicators]</t>
+  </si>
+  <si>
+    <t>Sharpe Ratio</t>
   </si>
 </sst>
 </file>
@@ -327,7 +330,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -446,22 +449,31 @@
     </border>
     <border>
       <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
       <right/>
       <top/>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -480,7 +492,7 @@
     <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="6"/>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="7"/>
@@ -495,6 +507,45 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="2" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" xfId="11" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="12" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" xfId="10" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" xfId="11" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" xfId="12" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="3" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="9" xfId="12" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" xfId="12" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="9" xfId="11" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" xfId="11" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="5" xfId="8" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -507,51 +558,17 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="6" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="3" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="10" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="11" xfId="7" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" xfId="10" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" xfId="12" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" xfId="11" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="9" xfId="11" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" xfId="11" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="9" xfId="12" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" xfId="12" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" xfId="11" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="13">
@@ -879,46 +896,47 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9BB286C-59E4-364D-813B-B93A3B7BF266}">
-  <dimension ref="A1:Q45"/>
+  <dimension ref="A1:R47"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A27" zoomScale="133" workbookViewId="0">
-      <selection activeCell="L32" sqref="L32"/>
+      <selection activeCell="R32" sqref="R32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="C1" s="8" t="s">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="C1" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
       <c r="F1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="H1" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="9"/>
-      <c r="J1" s="10" t="s">
+      <c r="I1" s="24"/>
+      <c r="J1" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="11"/>
-      <c r="L1" s="13" t="s">
+      <c r="K1" s="26"/>
+      <c r="L1" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="M1" s="14"/>
-      <c r="N1" s="14"/>
-      <c r="O1" s="12" t="s">
+      <c r="M1" s="28"/>
+      <c r="N1" s="28"/>
+      <c r="O1" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="P1" s="12"/>
-      <c r="Q1" s="12"/>
-    </row>
-    <row r="2" spans="1:17" ht="51" x14ac:dyDescent="0.2">
+      <c r="P1" s="30"/>
+      <c r="Q1" s="30"/>
+      <c r="R1" s="30"/>
+    </row>
+    <row r="2" spans="1:18" ht="51" x14ac:dyDescent="0.2">
       <c r="B2" s="3" t="s">
         <v>7</v>
       </c>
@@ -967,32 +985,36 @@
       <c r="Q2" s="5" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="3" spans="1:17" ht="29" x14ac:dyDescent="0.35">
-      <c r="A3" s="18" t="s">
+      <c r="R2" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" ht="29" x14ac:dyDescent="0.35">
+      <c r="A3" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="17"/>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="17"/>
-      <c r="G3" s="17"/>
-      <c r="H3" s="17"/>
-      <c r="I3" s="17"/>
-      <c r="J3" s="17"/>
-      <c r="K3" s="17"/>
-      <c r="L3" s="17"/>
-      <c r="M3" s="17"/>
-      <c r="N3" s="17"/>
-      <c r="O3" s="17"/>
-      <c r="P3" s="17"/>
-      <c r="Q3" s="17"/>
-    </row>
-    <row r="4" spans="1:17" ht="34" x14ac:dyDescent="0.2">
-      <c r="A4" s="18"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
+      <c r="I3" s="14"/>
+      <c r="J3" s="14"/>
+      <c r="K3" s="14"/>
+      <c r="L3" s="14"/>
+      <c r="M3" s="14"/>
+      <c r="N3" s="14"/>
+      <c r="O3" s="14"/>
+      <c r="P3" s="14"/>
+      <c r="Q3" s="14"/>
+      <c r="R3" s="14"/>
+    </row>
+    <row r="4" spans="1:18" ht="34" x14ac:dyDescent="0.2">
+      <c r="A4" s="15"/>
       <c r="B4" s="6">
         <v>1</v>
       </c>
@@ -1044,8 +1066,8 @@
         <v>2.11</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="69" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="18"/>
+    <row r="5" spans="1:18" ht="69" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="15"/>
       <c r="B5" s="6">
         <v>2</v>
       </c>
@@ -1097,27 +1119,27 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="18"/>
-      <c r="B6" s="15"/>
-      <c r="C6" s="15"/>
-      <c r="D6" s="15"/>
-      <c r="E6" s="15"/>
-      <c r="F6" s="15"/>
-      <c r="G6" s="15"/>
-      <c r="H6" s="15"/>
-      <c r="I6" s="15"/>
-      <c r="J6" s="15"/>
-      <c r="K6" s="15"/>
-      <c r="L6" s="15"/>
-      <c r="M6" s="15"/>
-      <c r="N6" s="15"/>
-      <c r="O6" s="15"/>
-      <c r="P6" s="15"/>
-      <c r="Q6" s="15"/>
-    </row>
-    <row r="7" spans="1:17" ht="35" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="18"/>
+    <row r="6" spans="1:18" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="15"/>
+      <c r="B6" s="18"/>
+      <c r="C6" s="18"/>
+      <c r="D6" s="18"/>
+      <c r="E6" s="18"/>
+      <c r="F6" s="18"/>
+      <c r="G6" s="18"/>
+      <c r="H6" s="18"/>
+      <c r="I6" s="18"/>
+      <c r="J6" s="18"/>
+      <c r="K6" s="18"/>
+      <c r="L6" s="18"/>
+      <c r="M6" s="18"/>
+      <c r="N6" s="18"/>
+      <c r="O6" s="18"/>
+      <c r="P6" s="18"/>
+      <c r="Q6" s="18"/>
+    </row>
+    <row r="7" spans="1:18" ht="35" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="15"/>
       <c r="B7" s="6">
         <v>3</v>
       </c>
@@ -1169,8 +1191,8 @@
         <v>2.16</v>
       </c>
     </row>
-    <row r="8" spans="1:17" ht="69" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="18"/>
+    <row r="8" spans="1:18" ht="69" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="15"/>
       <c r="B8" s="6">
         <v>4</v>
       </c>
@@ -1222,27 +1244,27 @@
         <v>0.82</v>
       </c>
     </row>
-    <row r="9" spans="1:17" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="18"/>
-      <c r="B9" s="15"/>
-      <c r="C9" s="15"/>
-      <c r="D9" s="15"/>
-      <c r="E9" s="15"/>
-      <c r="F9" s="15"/>
-      <c r="G9" s="15"/>
-      <c r="H9" s="15"/>
-      <c r="I9" s="15"/>
-      <c r="J9" s="15"/>
-      <c r="K9" s="15"/>
-      <c r="L9" s="15"/>
-      <c r="M9" s="15"/>
-      <c r="N9" s="15"/>
-      <c r="O9" s="15"/>
-      <c r="P9" s="15"/>
-      <c r="Q9" s="15"/>
-    </row>
-    <row r="10" spans="1:17" ht="35" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="18"/>
+    <row r="9" spans="1:18" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="15"/>
+      <c r="B9" s="18"/>
+      <c r="C9" s="18"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="18"/>
+      <c r="H9" s="18"/>
+      <c r="I9" s="18"/>
+      <c r="J9" s="18"/>
+      <c r="K9" s="18"/>
+      <c r="L9" s="18"/>
+      <c r="M9" s="18"/>
+      <c r="N9" s="18"/>
+      <c r="O9" s="18"/>
+      <c r="P9" s="18"/>
+      <c r="Q9" s="18"/>
+    </row>
+    <row r="10" spans="1:18" ht="35" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="15"/>
       <c r="B10" s="6">
         <v>5</v>
       </c>
@@ -1292,8 +1314,8 @@
         <v>0.85</v>
       </c>
     </row>
-    <row r="11" spans="1:17" ht="69" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="18"/>
+    <row r="11" spans="1:18" ht="69" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="15"/>
       <c r="B11" s="6">
         <v>6</v>
       </c>
@@ -1343,27 +1365,27 @@
         <v>0.27</v>
       </c>
     </row>
-    <row r="12" spans="1:17" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="18"/>
-      <c r="B12" s="15"/>
-      <c r="C12" s="15"/>
-      <c r="D12" s="15"/>
-      <c r="E12" s="15"/>
-      <c r="F12" s="15"/>
-      <c r="G12" s="15"/>
-      <c r="H12" s="15"/>
-      <c r="I12" s="15"/>
-      <c r="J12" s="15"/>
-      <c r="K12" s="15"/>
-      <c r="L12" s="15"/>
-      <c r="M12" s="15"/>
-      <c r="N12" s="15"/>
-      <c r="O12" s="15"/>
-      <c r="P12" s="15"/>
-      <c r="Q12" s="15"/>
-    </row>
-    <row r="13" spans="1:17" ht="35" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="18"/>
+    <row r="12" spans="1:18" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="15"/>
+      <c r="B12" s="18"/>
+      <c r="C12" s="18"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="18"/>
+      <c r="G12" s="18"/>
+      <c r="H12" s="18"/>
+      <c r="I12" s="18"/>
+      <c r="J12" s="18"/>
+      <c r="K12" s="18"/>
+      <c r="L12" s="18"/>
+      <c r="M12" s="18"/>
+      <c r="N12" s="18"/>
+      <c r="O12" s="18"/>
+      <c r="P12" s="18"/>
+      <c r="Q12" s="18"/>
+    </row>
+    <row r="13" spans="1:18" ht="35" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="15"/>
       <c r="B13" s="6">
         <v>7</v>
       </c>
@@ -1414,8 +1436,8 @@
         <v>2.3199999999999998</v>
       </c>
     </row>
-    <row r="14" spans="1:17" ht="69" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="18"/>
+    <row r="14" spans="1:18" ht="69" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="15"/>
       <c r="B14" s="6">
         <v>8</v>
       </c>
@@ -1465,27 +1487,27 @@
         <v>0.89</v>
       </c>
     </row>
-    <row r="15" spans="1:17" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="18"/>
-      <c r="B15" s="15"/>
-      <c r="C15" s="15"/>
-      <c r="D15" s="15"/>
-      <c r="E15" s="15"/>
-      <c r="F15" s="15"/>
-      <c r="G15" s="15"/>
-      <c r="H15" s="15"/>
-      <c r="I15" s="15"/>
-      <c r="J15" s="15"/>
-      <c r="K15" s="15"/>
-      <c r="L15" s="15"/>
-      <c r="M15" s="15"/>
-      <c r="N15" s="15"/>
-      <c r="O15" s="15"/>
-      <c r="P15" s="15"/>
-      <c r="Q15" s="15"/>
-    </row>
-    <row r="16" spans="1:17" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="20" t="s">
+    <row r="15" spans="1:18" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="15"/>
+      <c r="B15" s="18"/>
+      <c r="C15" s="18"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="18"/>
+      <c r="G15" s="18"/>
+      <c r="H15" s="18"/>
+      <c r="I15" s="18"/>
+      <c r="J15" s="18"/>
+      <c r="K15" s="18"/>
+      <c r="L15" s="18"/>
+      <c r="M15" s="18"/>
+      <c r="N15" s="18"/>
+      <c r="O15" s="18"/>
+      <c r="P15" s="18"/>
+      <c r="Q15" s="18"/>
+    </row>
+    <row r="16" spans="1:18" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="16" t="s">
         <v>29</v>
       </c>
       <c r="B16" s="21" t="s">
@@ -1507,8 +1529,8 @@
       <c r="P16" s="21"/>
       <c r="Q16" s="21"/>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A17" s="20"/>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A17" s="16"/>
       <c r="B17" s="22"/>
       <c r="C17" s="22"/>
       <c r="D17" s="22"/>
@@ -1526,8 +1548,8 @@
       <c r="P17" s="22"/>
       <c r="Q17" s="22"/>
     </row>
-    <row r="18" spans="1:17" ht="34" x14ac:dyDescent="0.2">
-      <c r="A18" s="20"/>
+    <row r="18" spans="1:18" ht="34" x14ac:dyDescent="0.2">
+      <c r="A18" s="16"/>
       <c r="B18" s="6">
         <v>1</v>
       </c>
@@ -1579,8 +1601,8 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="19" spans="1:17" ht="68" x14ac:dyDescent="0.2">
-      <c r="A19" s="20"/>
+    <row r="19" spans="1:18" ht="68" x14ac:dyDescent="0.2">
+      <c r="A19" s="16"/>
       <c r="B19" s="6">
         <v>2</v>
       </c>
@@ -1632,8 +1654,8 @@
         <v>1.1100000000000001</v>
       </c>
     </row>
-    <row r="20" spans="1:17" ht="86" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="20"/>
+    <row r="20" spans="1:18" ht="86" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="16"/>
       <c r="B20" s="6">
         <v>3</v>
       </c>
@@ -1646,7 +1668,7 @@
       <c r="E20" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="F20" s="26" t="s">
+      <c r="F20" s="10" t="s">
         <v>32</v>
       </c>
       <c r="G20" s="6">
@@ -1679,33 +1701,33 @@
         <v>10</v>
       </c>
       <c r="P20" s="6">
-        <v>-15</v>
+        <v>701.66</v>
       </c>
       <c r="Q20" s="6">
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="21" spans="1:17" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="20"/>
-      <c r="B21" s="15"/>
-      <c r="C21" s="15"/>
-      <c r="D21" s="15"/>
-      <c r="E21" s="15"/>
-      <c r="F21" s="15"/>
-      <c r="G21" s="15"/>
-      <c r="H21" s="15"/>
-      <c r="I21" s="15"/>
-      <c r="J21" s="15"/>
-      <c r="K21" s="15"/>
-      <c r="L21" s="15"/>
-      <c r="M21" s="15"/>
-      <c r="N21" s="15"/>
-      <c r="O21" s="15"/>
-      <c r="P21" s="15"/>
-      <c r="Q21" s="15"/>
-    </row>
-    <row r="22" spans="1:17" ht="35" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="20"/>
+        <v>1.28</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="16"/>
+      <c r="B21" s="18"/>
+      <c r="C21" s="18"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="18"/>
+      <c r="F21" s="18"/>
+      <c r="G21" s="18"/>
+      <c r="H21" s="18"/>
+      <c r="I21" s="18"/>
+      <c r="J21" s="18"/>
+      <c r="K21" s="18"/>
+      <c r="L21" s="18"/>
+      <c r="M21" s="18"/>
+      <c r="N21" s="18"/>
+      <c r="O21" s="18"/>
+      <c r="P21" s="18"/>
+      <c r="Q21" s="18"/>
+    </row>
+    <row r="22" spans="1:18" ht="35" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="16"/>
       <c r="B22" s="6">
         <v>1</v>
       </c>
@@ -1757,8 +1779,8 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="23" spans="1:17" ht="68" x14ac:dyDescent="0.2">
-      <c r="A23" s="20"/>
+    <row r="23" spans="1:18" ht="68" x14ac:dyDescent="0.2">
+      <c r="A23" s="16"/>
       <c r="B23" s="6">
         <v>2</v>
       </c>
@@ -1810,78 +1832,78 @@
         <v>3.04</v>
       </c>
     </row>
-    <row r="24" spans="1:17" ht="86" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="20"/>
-      <c r="B24" s="25">
+    <row r="24" spans="1:18" ht="86" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="16"/>
+      <c r="B24" s="9">
         <v>3</v>
       </c>
-      <c r="C24" s="26" t="s">
+      <c r="C24" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="D24" s="26" t="s">
+      <c r="D24" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="E24" s="26" t="s">
-        <v>20</v>
-      </c>
-      <c r="F24" s="26" t="s">
+      <c r="E24" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="F24" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="G24" s="25">
+      <c r="G24" s="9">
         <v>14</v>
       </c>
-      <c r="H24" s="25">
-        <v>2142</v>
-      </c>
-      <c r="I24" s="25">
-        <v>814</v>
-      </c>
-      <c r="J24" s="25" t="s">
+      <c r="H24" s="9">
+        <v>2142</v>
+      </c>
+      <c r="I24" s="9">
+        <v>814</v>
+      </c>
+      <c r="J24" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="K24" s="25" t="s">
-        <v>22</v>
-      </c>
-      <c r="L24" s="25">
+      <c r="K24" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="L24" s="9">
         <v>117</v>
       </c>
-      <c r="M24" s="25">
-        <v>2142</v>
-      </c>
-      <c r="N24" s="25">
+      <c r="M24" s="9">
+        <v>2142</v>
+      </c>
+      <c r="N24" s="9">
         <v>250000</v>
       </c>
-      <c r="O24" s="25">
-        <v>10</v>
-      </c>
-      <c r="P24" s="25">
-        <v>829</v>
-      </c>
-      <c r="Q24" s="25">
-        <v>4.12</v>
-      </c>
-    </row>
-    <row r="25" spans="1:17" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="20"/>
-      <c r="B25" s="15"/>
-      <c r="C25" s="15"/>
-      <c r="D25" s="15"/>
-      <c r="E25" s="15"/>
-      <c r="F25" s="15"/>
-      <c r="G25" s="15"/>
-      <c r="H25" s="15"/>
-      <c r="I25" s="15"/>
-      <c r="J25" s="15"/>
-      <c r="K25" s="15"/>
-      <c r="L25" s="15"/>
-      <c r="M25" s="15"/>
-      <c r="N25" s="15"/>
-      <c r="O25" s="15"/>
-      <c r="P25" s="15"/>
-      <c r="Q25" s="15"/>
-    </row>
-    <row r="26" spans="1:17" ht="35" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="20"/>
+      <c r="O24" s="9">
+        <v>10</v>
+      </c>
+      <c r="P24" s="9">
+        <v>469.77</v>
+      </c>
+      <c r="Q24" s="9">
+        <v>5.26</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="16"/>
+      <c r="B25" s="18"/>
+      <c r="C25" s="18"/>
+      <c r="D25" s="18"/>
+      <c r="E25" s="18"/>
+      <c r="F25" s="18"/>
+      <c r="G25" s="18"/>
+      <c r="H25" s="18"/>
+      <c r="I25" s="18"/>
+      <c r="J25" s="18"/>
+      <c r="K25" s="18"/>
+      <c r="L25" s="18"/>
+      <c r="M25" s="18"/>
+      <c r="N25" s="18"/>
+      <c r="O25" s="18"/>
+      <c r="P25" s="18"/>
+      <c r="Q25" s="18"/>
+    </row>
+    <row r="26" spans="1:18" ht="35" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="16"/>
       <c r="B26" s="6">
         <v>1</v>
       </c>
@@ -1931,8 +1953,8 @@
         <v>1.0049999999999999</v>
       </c>
     </row>
-    <row r="27" spans="1:17" ht="68" x14ac:dyDescent="0.2">
-      <c r="A27" s="20"/>
+    <row r="27" spans="1:18" ht="68" x14ac:dyDescent="0.2">
+      <c r="A27" s="16"/>
       <c r="B27" s="6">
         <v>2</v>
       </c>
@@ -1982,78 +2004,78 @@
         <v>12.65</v>
       </c>
     </row>
-    <row r="28" spans="1:17" ht="86" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="20"/>
-      <c r="B28" s="25">
+    <row r="28" spans="1:18" ht="86" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="16"/>
+      <c r="B28" s="9">
         <v>3</v>
       </c>
-      <c r="C28" s="26" t="s">
+      <c r="C28" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="D28" s="26" t="s">
+      <c r="D28" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="E28" s="26" t="s">
-        <v>20</v>
-      </c>
-      <c r="F28" s="26" t="s">
+      <c r="E28" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="F28" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="G28" s="25">
-        <v>20</v>
-      </c>
-      <c r="H28" s="25">
-        <v>2142</v>
-      </c>
-      <c r="I28" s="25">
-        <v>814</v>
-      </c>
-      <c r="J28" s="25" t="s">
+      <c r="G28" s="9">
+        <v>20</v>
+      </c>
+      <c r="H28" s="9">
+        <v>2142</v>
+      </c>
+      <c r="I28" s="9">
+        <v>814</v>
+      </c>
+      <c r="J28" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="K28" s="25" t="s">
-        <v>22</v>
-      </c>
-      <c r="L28" s="25">
+      <c r="K28" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="L28" s="9">
         <v>117</v>
       </c>
-      <c r="M28" s="25">
-        <v>2142</v>
-      </c>
-      <c r="N28" s="25">
+      <c r="M28" s="9">
+        <v>2142</v>
+      </c>
+      <c r="N28" s="9">
         <v>250000</v>
       </c>
-      <c r="O28" s="25">
-        <v>10</v>
-      </c>
-      <c r="P28" s="25">
+      <c r="O28" s="9">
+        <v>10</v>
+      </c>
+      <c r="P28" s="9">
         <v>122.61</v>
       </c>
-      <c r="Q28" s="25">
+      <c r="Q28" s="9">
         <v>1.06</v>
       </c>
     </row>
-    <row r="29" spans="1:17" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="20"/>
-      <c r="B29" s="15"/>
-      <c r="C29" s="15"/>
-      <c r="D29" s="15"/>
-      <c r="E29" s="15"/>
-      <c r="F29" s="15"/>
-      <c r="G29" s="15"/>
-      <c r="H29" s="15"/>
-      <c r="I29" s="15"/>
-      <c r="J29" s="15"/>
-      <c r="K29" s="15"/>
-      <c r="L29" s="15"/>
-      <c r="M29" s="15"/>
-      <c r="N29" s="15"/>
-      <c r="O29" s="15"/>
-      <c r="P29" s="15"/>
-      <c r="Q29" s="15"/>
-    </row>
-    <row r="30" spans="1:17" ht="35" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="20"/>
+    <row r="29" spans="1:18" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="16"/>
+      <c r="B29" s="18"/>
+      <c r="C29" s="18"/>
+      <c r="D29" s="18"/>
+      <c r="E29" s="18"/>
+      <c r="F29" s="18"/>
+      <c r="G29" s="18"/>
+      <c r="H29" s="18"/>
+      <c r="I29" s="18"/>
+      <c r="J29" s="18"/>
+      <c r="K29" s="18"/>
+      <c r="L29" s="18"/>
+      <c r="M29" s="18"/>
+      <c r="N29" s="18"/>
+      <c r="O29" s="18"/>
+      <c r="P29" s="18"/>
+      <c r="Q29" s="18"/>
+    </row>
+    <row r="30" spans="1:18" ht="35" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="16"/>
       <c r="B30" s="6">
         <v>1</v>
       </c>
@@ -2104,8 +2126,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:17" ht="68" x14ac:dyDescent="0.2">
-      <c r="A31" s="20"/>
+    <row r="31" spans="1:18" ht="68" x14ac:dyDescent="0.2">
+      <c r="A31" s="16"/>
       <c r="B31" s="6">
         <v>2</v>
       </c>
@@ -2154,244 +2176,282 @@
       <c r="Q31" s="6">
         <v>13</v>
       </c>
-    </row>
-    <row r="32" spans="1:17" ht="86" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="27"/>
-      <c r="B32" s="25">
+      <c r="R31" s="11">
+        <v>1.43</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18" ht="85" x14ac:dyDescent="0.2">
+      <c r="A32" s="8"/>
+      <c r="B32" s="9">
         <v>3</v>
       </c>
-      <c r="C32" s="26" t="s">
+      <c r="C32" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="D32" s="26" t="s">
+      <c r="D32" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="E32" s="26" t="s">
-        <v>20</v>
-      </c>
-      <c r="F32" s="26" t="s">
+      <c r="E32" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="F32" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="G32" s="25">
+      <c r="G32" s="9">
         <v>14</v>
       </c>
-      <c r="H32" s="25">
-        <v>2142</v>
-      </c>
-      <c r="I32" s="25">
-        <v>814</v>
-      </c>
-      <c r="J32" s="25" t="s">
+      <c r="H32" s="9">
+        <v>2142</v>
+      </c>
+      <c r="I32" s="9">
+        <v>814</v>
+      </c>
+      <c r="J32" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="K32" s="25" t="s">
+      <c r="K32" s="9" t="s">
         <v>22</v>
       </c>
       <c r="L32" s="6">
         <v>467</v>
       </c>
-      <c r="M32" s="25">
-        <v>2142</v>
-      </c>
-      <c r="N32" s="25">
+      <c r="M32" s="9">
+        <v>2142</v>
+      </c>
+      <c r="N32" s="9">
         <v>1000000</v>
       </c>
-      <c r="O32" s="25">
-        <v>10</v>
-      </c>
-      <c r="P32" s="25">
+      <c r="O32" s="9">
+        <v>10</v>
+      </c>
+      <c r="P32" s="9">
         <v>15.7</v>
       </c>
-      <c r="Q32" s="25">
+      <c r="Q32" s="9">
         <v>17.440000000000001</v>
       </c>
-    </row>
-    <row r="33" spans="1:17" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="19" t="s">
+      <c r="R32" s="12">
+        <v>2.41</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17" ht="85" x14ac:dyDescent="0.2">
+      <c r="A33" s="8"/>
+      <c r="B33" s="9">
+        <v>4</v>
+      </c>
+      <c r="C33" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D33" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="E33" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="F33" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="G33" s="9">
+        <v>14</v>
+      </c>
+      <c r="H33" s="9">
+        <v>2142</v>
+      </c>
+      <c r="I33" s="9">
+        <v>814</v>
+      </c>
+      <c r="J33" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="K33" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="L33" s="6">
+        <f>ROUND(N33/H33,0)</f>
+        <v>934</v>
+      </c>
+      <c r="M33" s="9">
+        <v>2142</v>
+      </c>
+      <c r="N33" s="9">
+        <v>2000000</v>
+      </c>
+      <c r="O33" s="9">
+        <v>10</v>
+      </c>
+      <c r="P33" s="9">
+        <v>715.9</v>
+      </c>
+      <c r="Q33" s="9">
+        <v>15.9</v>
+      </c>
+    </row>
+    <row r="34" spans="1:17" ht="86" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="8"/>
+      <c r="B34" s="9">
+        <v>5</v>
+      </c>
+      <c r="C34" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D34" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="E34" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="F34" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="G34" s="9">
+        <v>14</v>
+      </c>
+      <c r="H34" s="9">
+        <v>2142</v>
+      </c>
+      <c r="I34" s="9">
+        <v>814</v>
+      </c>
+      <c r="J34" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="K34" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="L34" s="6">
+        <f>ROUND(N34/H34,0)</f>
+        <v>1401</v>
+      </c>
+      <c r="M34" s="9">
+        <v>2142</v>
+      </c>
+      <c r="N34" s="9">
+        <v>3000000</v>
+      </c>
+      <c r="O34" s="9">
+        <v>10</v>
+      </c>
+      <c r="P34" s="9">
+        <v>-14.88</v>
+      </c>
+      <c r="Q34" s="9">
+        <v>17.04</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="B33" s="23" t="s">
+      <c r="B35" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="C33" s="23"/>
-      <c r="D33" s="23"/>
-      <c r="E33" s="23"/>
-      <c r="F33" s="23"/>
-      <c r="G33" s="23"/>
-      <c r="H33" s="23"/>
-      <c r="I33" s="23"/>
-      <c r="J33" s="23"/>
-      <c r="K33" s="23"/>
-      <c r="L33" s="23"/>
-      <c r="M33" s="23"/>
-      <c r="N33" s="23"/>
-      <c r="O33" s="23"/>
-      <c r="P33" s="23"/>
-      <c r="Q33" s="23"/>
-    </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A34" s="19"/>
-      <c r="B34" s="24"/>
-      <c r="C34" s="24"/>
-      <c r="D34" s="24"/>
-      <c r="E34" s="24"/>
-      <c r="F34" s="24"/>
-      <c r="G34" s="24"/>
-      <c r="H34" s="24"/>
-      <c r="I34" s="24"/>
-      <c r="J34" s="24"/>
-      <c r="K34" s="24"/>
-      <c r="L34" s="24"/>
-      <c r="M34" s="24"/>
-      <c r="N34" s="24"/>
-      <c r="O34" s="24"/>
-      <c r="P34" s="24"/>
-      <c r="Q34" s="24"/>
-    </row>
-    <row r="35" spans="1:17" ht="34" x14ac:dyDescent="0.2">
-      <c r="A35" s="19"/>
-      <c r="B35" s="6">
+      <c r="C35" s="19"/>
+      <c r="D35" s="19"/>
+      <c r="E35" s="19"/>
+      <c r="F35" s="19"/>
+      <c r="G35" s="19"/>
+      <c r="H35" s="19"/>
+      <c r="I35" s="19"/>
+      <c r="J35" s="19"/>
+      <c r="K35" s="19"/>
+      <c r="L35" s="19"/>
+      <c r="M35" s="19"/>
+      <c r="N35" s="19"/>
+      <c r="O35" s="19"/>
+      <c r="P35" s="19"/>
+      <c r="Q35" s="19"/>
+    </row>
+    <row r="36" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A36" s="17"/>
+      <c r="B36" s="20"/>
+      <c r="C36" s="20"/>
+      <c r="D36" s="20"/>
+      <c r="E36" s="20"/>
+      <c r="F36" s="20"/>
+      <c r="G36" s="20"/>
+      <c r="H36" s="20"/>
+      <c r="I36" s="20"/>
+      <c r="J36" s="20"/>
+      <c r="K36" s="20"/>
+      <c r="L36" s="20"/>
+      <c r="M36" s="20"/>
+      <c r="N36" s="20"/>
+      <c r="O36" s="20"/>
+      <c r="P36" s="20"/>
+      <c r="Q36" s="20"/>
+    </row>
+    <row r="37" spans="1:17" ht="34" x14ac:dyDescent="0.2">
+      <c r="A37" s="17"/>
+      <c r="B37" s="6">
         <v>1</v>
       </c>
-      <c r="C35" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D35" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="E35" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="F35" s="7" t="s">
+      <c r="C37" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D37" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E37" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F37" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="G35" s="6">
+      <c r="G37" s="6">
         <v>9</v>
       </c>
-      <c r="H35" s="6">
-        <v>2142</v>
-      </c>
-      <c r="I35" s="6">
-        <v>814</v>
-      </c>
-      <c r="J35" s="6" t="s">
+      <c r="H37" s="6">
+        <v>2142</v>
+      </c>
+      <c r="I37" s="6">
+        <v>814</v>
+      </c>
+      <c r="J37" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="K35" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="L35" s="6">
-        <f>ROUND(N35/H35,0)</f>
+      <c r="K37" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="L37" s="6">
+        <f>ROUND(N37/H37,0)</f>
         <v>117</v>
       </c>
-      <c r="M35" s="6">
-        <f>H35</f>
-        <v>2142</v>
-      </c>
-      <c r="N35" s="6">
+      <c r="M37" s="6">
+        <f>H37</f>
+        <v>2142</v>
+      </c>
+      <c r="N37" s="6">
         <v>250000</v>
       </c>
-      <c r="O35" s="6">
-        <v>10</v>
-      </c>
-      <c r="P35" s="6">
+      <c r="O37" s="6">
+        <v>10</v>
+      </c>
+      <c r="P37" s="6">
         <v>782</v>
       </c>
-      <c r="Q35" s="6">
+      <c r="Q37" s="6">
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="36" spans="1:17" ht="69" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="19"/>
-      <c r="B36" s="6">
+    <row r="38" spans="1:17" ht="69" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="17"/>
+      <c r="B38" s="6">
         <v>2</v>
       </c>
-      <c r="C36" s="7" t="s">
+      <c r="C38" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="D36" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="E36" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="F36" s="7" t="s">
+      <c r="D38" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E38" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F38" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="G36" s="6">
+      <c r="G38" s="6">
         <v>9</v>
-      </c>
-      <c r="H36" s="6">
-        <v>2142</v>
-      </c>
-      <c r="I36" s="6">
-        <v>814</v>
-      </c>
-      <c r="J36" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="K36" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="L36" s="6">
-        <f>ROUND(N36/H36,0)</f>
-        <v>117</v>
-      </c>
-      <c r="M36" s="6">
-        <f>H36</f>
-        <v>2142</v>
-      </c>
-      <c r="N36" s="6">
-        <v>250000</v>
-      </c>
-      <c r="O36" s="6">
-        <v>10</v>
-      </c>
-      <c r="P36" s="6">
-        <v>-75</v>
-      </c>
-      <c r="Q36" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:17" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="19"/>
-      <c r="B37" s="15"/>
-      <c r="C37" s="15"/>
-      <c r="D37" s="15"/>
-      <c r="E37" s="15"/>
-      <c r="F37" s="15"/>
-      <c r="G37" s="15"/>
-      <c r="H37" s="15"/>
-      <c r="I37" s="15"/>
-      <c r="J37" s="15"/>
-      <c r="K37" s="15"/>
-      <c r="L37" s="15"/>
-      <c r="M37" s="15"/>
-      <c r="N37" s="15"/>
-      <c r="O37" s="15"/>
-      <c r="P37" s="15"/>
-      <c r="Q37" s="15"/>
-    </row>
-    <row r="38" spans="1:17" ht="35" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="19"/>
-      <c r="B38" s="6">
-        <v>3</v>
-      </c>
-      <c r="C38" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D38" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="E38" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="F38" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="G38" s="6">
-        <v>14</v>
       </c>
       <c r="H38" s="6">
         <v>2142</v>
@@ -2420,103 +2480,103 @@
         <v>10</v>
       </c>
       <c r="P38" s="6">
+        <v>-75</v>
+      </c>
+      <c r="Q38" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:17" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="17"/>
+      <c r="B39" s="18"/>
+      <c r="C39" s="18"/>
+      <c r="D39" s="18"/>
+      <c r="E39" s="18"/>
+      <c r="F39" s="18"/>
+      <c r="G39" s="18"/>
+      <c r="H39" s="18"/>
+      <c r="I39" s="18"/>
+      <c r="J39" s="18"/>
+      <c r="K39" s="18"/>
+      <c r="L39" s="18"/>
+      <c r="M39" s="18"/>
+      <c r="N39" s="18"/>
+      <c r="O39" s="18"/>
+      <c r="P39" s="18"/>
+      <c r="Q39" s="18"/>
+    </row>
+    <row r="40" spans="1:17" ht="35" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="17"/>
+      <c r="B40" s="6">
+        <v>3</v>
+      </c>
+      <c r="C40" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D40" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E40" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F40" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="G40" s="6">
+        <v>14</v>
+      </c>
+      <c r="H40" s="6">
+        <v>2142</v>
+      </c>
+      <c r="I40" s="6">
+        <v>814</v>
+      </c>
+      <c r="J40" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="K40" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="L40" s="6">
+        <f>ROUND(N40/H40,0)</f>
+        <v>117</v>
+      </c>
+      <c r="M40" s="6">
+        <f>H40</f>
+        <v>2142</v>
+      </c>
+      <c r="N40" s="6">
+        <v>250000</v>
+      </c>
+      <c r="O40" s="6">
+        <v>10</v>
+      </c>
+      <c r="P40" s="6">
         <v>414.99</v>
       </c>
-      <c r="Q38" s="6">
+      <c r="Q40" s="6">
         <v>0.19</v>
       </c>
     </row>
-    <row r="39" spans="1:17" ht="69" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="19"/>
-      <c r="B39" s="6">
+    <row r="41" spans="1:17" ht="69" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="17"/>
+      <c r="B41" s="6">
         <v>4</v>
       </c>
-      <c r="C39" s="7" t="s">
+      <c r="C41" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="D39" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="E39" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="F39" s="7" t="s">
+      <c r="D41" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E41" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F41" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="G39" s="6">
+      <c r="G41" s="6">
         <v>14</v>
-      </c>
-      <c r="H39" s="6">
-        <v>2142</v>
-      </c>
-      <c r="I39" s="6">
-        <v>814</v>
-      </c>
-      <c r="J39" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="K39" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="L39" s="6">
-        <f>ROUND(N39/H39,0)</f>
-        <v>117</v>
-      </c>
-      <c r="M39" s="6">
-        <f>H39</f>
-        <v>2142</v>
-      </c>
-      <c r="N39" s="6">
-        <v>250000</v>
-      </c>
-      <c r="O39" s="6">
-        <v>10</v>
-      </c>
-      <c r="P39" s="6">
-        <v>716.66</v>
-      </c>
-      <c r="Q39" s="6">
-        <v>6.2</v>
-      </c>
-    </row>
-    <row r="40" spans="1:17" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="19"/>
-      <c r="B40" s="15"/>
-      <c r="C40" s="15"/>
-      <c r="D40" s="15"/>
-      <c r="E40" s="15"/>
-      <c r="F40" s="15"/>
-      <c r="G40" s="15"/>
-      <c r="H40" s="15"/>
-      <c r="I40" s="15"/>
-      <c r="J40" s="15"/>
-      <c r="K40" s="15"/>
-      <c r="L40" s="15"/>
-      <c r="M40" s="15"/>
-      <c r="N40" s="15"/>
-      <c r="O40" s="15"/>
-      <c r="P40" s="15"/>
-      <c r="Q40" s="15"/>
-    </row>
-    <row r="41" spans="1:17" ht="35" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="19"/>
-      <c r="B41" s="6">
-        <v>5</v>
-      </c>
-      <c r="C41" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D41" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="E41" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="F41" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="G41" s="6">
-        <v>20</v>
       </c>
       <c r="H41" s="6">
         <v>2142</v>
@@ -2531,9 +2591,11 @@
         <v>22</v>
       </c>
       <c r="L41" s="6">
+        <f>ROUND(N41/H41,0)</f>
         <v>117</v>
       </c>
       <c r="M41" s="6">
+        <f>H41</f>
         <v>2142</v>
       </c>
       <c r="N41" s="6">
@@ -2543,101 +2605,101 @@
         <v>10</v>
       </c>
       <c r="P41" s="6">
+        <v>716.66</v>
+      </c>
+      <c r="Q41" s="6">
+        <v>6.2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:17" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="17"/>
+      <c r="B42" s="18"/>
+      <c r="C42" s="18"/>
+      <c r="D42" s="18"/>
+      <c r="E42" s="18"/>
+      <c r="F42" s="18"/>
+      <c r="G42" s="18"/>
+      <c r="H42" s="18"/>
+      <c r="I42" s="18"/>
+      <c r="J42" s="18"/>
+      <c r="K42" s="18"/>
+      <c r="L42" s="18"/>
+      <c r="M42" s="18"/>
+      <c r="N42" s="18"/>
+      <c r="O42" s="18"/>
+      <c r="P42" s="18"/>
+      <c r="Q42" s="18"/>
+    </row>
+    <row r="43" spans="1:17" ht="35" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="17"/>
+      <c r="B43" s="6">
+        <v>5</v>
+      </c>
+      <c r="C43" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D43" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E43" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F43" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="G43" s="6">
+        <v>20</v>
+      </c>
+      <c r="H43" s="6">
+        <v>2142</v>
+      </c>
+      <c r="I43" s="6">
+        <v>814</v>
+      </c>
+      <c r="J43" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="K43" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="L43" s="6">
+        <v>117</v>
+      </c>
+      <c r="M43" s="6">
+        <v>2142</v>
+      </c>
+      <c r="N43" s="6">
+        <v>250000</v>
+      </c>
+      <c r="O43" s="6">
+        <v>10</v>
+      </c>
+      <c r="P43" s="6">
         <v>540</v>
       </c>
-      <c r="Q41" s="6">
+      <c r="Q43" s="6">
         <v>0.33</v>
       </c>
     </row>
-    <row r="42" spans="1:17" ht="69" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="19"/>
-      <c r="B42" s="6">
+    <row r="44" spans="1:17" ht="69" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="17"/>
+      <c r="B44" s="6">
         <v>6</v>
       </c>
-      <c r="C42" s="7" t="s">
+      <c r="C44" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="D42" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="E42" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="F42" s="7" t="s">
+      <c r="D44" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E44" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F44" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="G42" s="6">
-        <v>20</v>
-      </c>
-      <c r="H42" s="6">
-        <v>2142</v>
-      </c>
-      <c r="I42" s="6">
-        <v>814</v>
-      </c>
-      <c r="J42" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="K42" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="L42" s="6">
-        <v>117</v>
-      </c>
-      <c r="M42" s="6">
-        <v>2142</v>
-      </c>
-      <c r="N42" s="6">
-        <v>250000</v>
-      </c>
-      <c r="O42" s="6">
-        <v>10</v>
-      </c>
-      <c r="P42" s="6">
-        <v>173</v>
-      </c>
-      <c r="Q42" s="6">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="43" spans="1:17" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="19"/>
-      <c r="B43" s="15"/>
-      <c r="C43" s="15"/>
-      <c r="D43" s="15"/>
-      <c r="E43" s="15"/>
-      <c r="F43" s="15"/>
-      <c r="G43" s="15"/>
-      <c r="H43" s="15"/>
-      <c r="I43" s="15"/>
-      <c r="J43" s="15"/>
-      <c r="K43" s="15"/>
-      <c r="L43" s="15"/>
-      <c r="M43" s="15"/>
-      <c r="N43" s="15"/>
-      <c r="O43" s="15"/>
-      <c r="P43" s="15"/>
-      <c r="Q43" s="15"/>
-    </row>
-    <row r="44" spans="1:17" ht="35" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="19"/>
-      <c r="B44" s="6">
-        <v>7</v>
-      </c>
-      <c r="C44" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D44" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="E44" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="F44" s="7" t="s">
-        <v>24</v>
-      </c>
       <c r="G44" s="6">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="H44" s="6">
         <v>2142</v>
@@ -2652,99 +2714,169 @@
         <v>22</v>
       </c>
       <c r="L44" s="6">
-        <f>ROUND(N44/H44,0)</f>
+        <v>117</v>
+      </c>
+      <c r="M44" s="6">
+        <v>2142</v>
+      </c>
+      <c r="N44" s="6">
+        <v>250000</v>
+      </c>
+      <c r="O44" s="6">
+        <v>10</v>
+      </c>
+      <c r="P44" s="6">
+        <v>173</v>
+      </c>
+      <c r="Q44" s="6">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="45" spans="1:17" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="17"/>
+      <c r="B45" s="18"/>
+      <c r="C45" s="18"/>
+      <c r="D45" s="18"/>
+      <c r="E45" s="18"/>
+      <c r="F45" s="18"/>
+      <c r="G45" s="18"/>
+      <c r="H45" s="18"/>
+      <c r="I45" s="18"/>
+      <c r="J45" s="18"/>
+      <c r="K45" s="18"/>
+      <c r="L45" s="18"/>
+      <c r="M45" s="18"/>
+      <c r="N45" s="18"/>
+      <c r="O45" s="18"/>
+      <c r="P45" s="18"/>
+      <c r="Q45" s="18"/>
+    </row>
+    <row r="46" spans="1:17" ht="35" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="17"/>
+      <c r="B46" s="6">
+        <v>7</v>
+      </c>
+      <c r="C46" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D46" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E46" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F46" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="G46" s="6">
+        <v>14</v>
+      </c>
+      <c r="H46" s="6">
+        <v>2142</v>
+      </c>
+      <c r="I46" s="6">
+        <v>814</v>
+      </c>
+      <c r="J46" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="K46" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="L46" s="6">
+        <f>ROUND(N46/H46,0)</f>
         <v>467</v>
       </c>
-      <c r="M44" s="6">
-        <v>2142</v>
-      </c>
-      <c r="N44" s="6">
+      <c r="M46" s="6">
+        <v>2142</v>
+      </c>
+      <c r="N46" s="6">
         <v>1000000</v>
       </c>
-      <c r="O44" s="6">
-        <v>10</v>
-      </c>
-      <c r="P44" s="6">
+      <c r="O46" s="6">
+        <v>10</v>
+      </c>
+      <c r="P46" s="6">
         <v>550</v>
       </c>
-      <c r="Q44" s="6">
+      <c r="Q46" s="6">
         <v>0.25</v>
       </c>
     </row>
-    <row r="45" spans="1:17" ht="68" x14ac:dyDescent="0.2">
-      <c r="A45" s="19"/>
-      <c r="B45" s="6">
+    <row r="47" spans="1:17" ht="68" x14ac:dyDescent="0.2">
+      <c r="A47" s="17"/>
+      <c r="B47" s="6">
         <v>8</v>
       </c>
-      <c r="C45" s="7" t="s">
+      <c r="C47" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="D45" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="E45" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="F45" s="7" t="s">
+      <c r="D47" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E47" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F47" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="G45" s="6">
+      <c r="G47" s="6">
         <v>14</v>
       </c>
-      <c r="H45" s="6">
-        <v>2142</v>
-      </c>
-      <c r="I45" s="6">
-        <v>814</v>
-      </c>
-      <c r="J45" s="6" t="s">
+      <c r="H47" s="6">
+        <v>2142</v>
+      </c>
+      <c r="I47" s="6">
+        <v>814</v>
+      </c>
+      <c r="J47" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="K45" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="L45" s="6">
+      <c r="K47" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="L47" s="6">
         <v>467</v>
       </c>
-      <c r="M45" s="6">
-        <v>2142</v>
-      </c>
-      <c r="N45" s="6">
+      <c r="M47" s="6">
+        <v>2142</v>
+      </c>
+      <c r="N47" s="6">
         <v>1000000</v>
       </c>
-      <c r="O45" s="6">
-        <v>10</v>
-      </c>
-      <c r="P45" s="6">
+      <c r="O47" s="6">
+        <v>10</v>
+      </c>
+      <c r="P47" s="6">
         <v>729</v>
       </c>
-      <c r="Q45" s="6">
+      <c r="Q47" s="6">
         <v>4.42</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="C1:E1"/>
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="L1:N1"/>
+    <mergeCell ref="O1:R1"/>
+    <mergeCell ref="B3:R3"/>
     <mergeCell ref="A3:A15"/>
     <mergeCell ref="A16:A31"/>
-    <mergeCell ref="A33:A45"/>
-    <mergeCell ref="B3:Q3"/>
+    <mergeCell ref="A35:A47"/>
     <mergeCell ref="B25:Q25"/>
     <mergeCell ref="B29:Q29"/>
-    <mergeCell ref="B33:Q34"/>
-    <mergeCell ref="B37:Q37"/>
-    <mergeCell ref="B40:Q40"/>
-    <mergeCell ref="B43:Q43"/>
+    <mergeCell ref="B35:Q36"/>
+    <mergeCell ref="B39:Q39"/>
+    <mergeCell ref="B42:Q42"/>
+    <mergeCell ref="B45:Q45"/>
     <mergeCell ref="B6:Q6"/>
     <mergeCell ref="B9:Q9"/>
     <mergeCell ref="B12:Q12"/>
     <mergeCell ref="B15:Q15"/>
     <mergeCell ref="B16:Q17"/>
     <mergeCell ref="B21:Q21"/>
-    <mergeCell ref="C1:E1"/>
-    <mergeCell ref="H1:I1"/>
-    <mergeCell ref="J1:K1"/>
-    <mergeCell ref="O1:Q1"/>
-    <mergeCell ref="L1:N1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>

</xml_diff>